<commit_message>
[SAI - Atenciones] Se corrigen las páginas de atención presencial y por correos, se agregan consultas de creación de tabla distribuida. [SAI] Se corrige validación de tipos de pqrs no existentes: 0 - {sin definir}.
</commit_message>
<xml_diff>
--- a/Documentación/Estructura_DB_30_SAI_solicitudes_presencial.xlsx
+++ b/Documentación/Estructura_DB_30_SAI_solicitudes_presencial.xlsx
@@ -29,10 +29,8 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -69,10 +67,8 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -124,10 +120,8 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -151,10 +145,8 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -179,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="109">
   <si>
     <t xml:space="preserve">App</t>
   </si>
@@ -503,6 +495,9 @@
   </si>
   <si>
     <t xml:space="preserve">saiu20idcaso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saiu21respuesta</t>
   </si>
 </sst>
 </file>
@@ -512,11 +507,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -556,8 +552,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -569,15 +566,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -588,6 +578,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB3A2C7"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -643,40 +645,56 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -690,6 +708,37 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Normal_Hoja2" xfId="20"/>
   </cellStyles>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB3A2C7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -734,7 +783,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -754,17 +803,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.43"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -819,31 +871,31 @@
       <c r="B2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="10" t="n">
         <v>3021</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="10" t="n">
         <v>3001</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -852,16 +904,16 @@
       <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="C3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -870,29 +922,29 @@
       <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="C4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="K4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M4" s="0" t="n">
+      <c r="H4" s="9"/>
+      <c r="K4" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="L4" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -900,16 +952,16 @@
       <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5" s="10" t="n">
         <v>6</v>
       </c>
     </row>
@@ -917,61 +969,61 @@
       <c r="B6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="8" t="s">
+      <c r="C6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6" s="10" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="K7" s="0" t="n">
+      <c r="C7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="K7" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="10" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="K8" s="0" t="n">
+      <c r="C8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="K8" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M8" s="10" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="K9" s="0" t="n">
+      <c r="C9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="K9" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9" s="10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -979,10 +1031,10 @@
       <c r="B10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="0" t="n">
+      <c r="C10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="10" t="n">
         <v>9</v>
       </c>
     </row>
@@ -990,14 +1042,14 @@
       <c r="B11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="K11" s="0" t="n">
+      <c r="C11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="K11" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="10" t="n">
         <v>71</v>
       </c>
     </row>
@@ -1005,13 +1057,13 @@
       <c r="B12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="0" t="n">
+      <c r="C12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12" s="10" t="n">
         <v>72</v>
       </c>
     </row>
@@ -1019,48 +1071,48 @@
       <c r="B13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="0" t="n">
+      <c r="C13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="L13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M13" s="0" t="n">
+      <c r="L13" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M13" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="N13" s="0" t="s">
+      <c r="N13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="O13" s="0" t="s">
+      <c r="O13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="P13" s="0" t="s">
+      <c r="P13" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="0" t="n">
+      <c r="C14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="L14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N14" s="0" t="s">
+      <c r="L14" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="N14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="O14" s="0" t="s">
+      <c r="O14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="P14" s="0" t="s">
+      <c r="P14" s="10" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1068,13 +1120,13 @@
       <c r="B15" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="0" t="n">
+      <c r="C15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15" s="10" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1082,22 +1134,22 @@
       <c r="B16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N16" s="0" t="s">
+      <c r="C16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="L16" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="N16" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="O16" s="0" t="s">
+      <c r="O16" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="P16" s="0" t="s">
+      <c r="P16" s="10" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1105,25 +1157,25 @@
       <c r="B17" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="0" t="n">
+      <c r="C17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="L17" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M17" s="0" t="n">
+      <c r="L17" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M17" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="N17" s="0" t="s">
+      <c r="N17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="O17" s="0" t="s">
+      <c r="O17" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="P17" s="0" t="s">
+      <c r="P17" s="10" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1131,22 +1183,22 @@
       <c r="B18" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" s="0" t="n">
+      <c r="C18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="L18" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N18" s="0" t="s">
+      <c r="L18" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="N18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="O18" s="0" t="s">
+      <c r="O18" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="P18" s="0" t="s">
+      <c r="P18" s="10" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1154,22 +1206,22 @@
       <c r="B19" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="0" t="n">
+      <c r="C19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="L19" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N19" s="0" t="s">
+      <c r="L19" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="N19" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="O19" s="0" t="s">
+      <c r="O19" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="P19" s="0" t="s">
+      <c r="P19" s="10" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1177,22 +1229,22 @@
       <c r="B20" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="0" t="n">
+      <c r="C20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="L20" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N20" s="0" t="s">
+      <c r="L20" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="N20" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="O20" s="0" t="s">
+      <c r="O20" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="P20" s="0" t="s">
+      <c r="P20" s="10" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1200,31 +1252,31 @@
       <c r="B21" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="0" t="n">
+      <c r="C21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="L21" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M21" s="0" t="n">
+      <c r="L21" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M21" s="10" t="n">
         <v>31</v>
       </c>
-      <c r="N21" s="0" t="s">
+      <c r="N21" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="O21" s="0" t="s">
+      <c r="O21" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="P21" s="0" t="s">
+      <c r="P21" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="Q21" s="0" t="s">
+      <c r="Q21" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="R21" s="0" t="n">
+      <c r="R21" s="10" t="n">
         <v>19</v>
       </c>
     </row>
@@ -1232,25 +1284,25 @@
       <c r="B22" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K22" s="0" t="n">
+      <c r="D22" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="K22" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="L22" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N22" s="0" t="s">
+      <c r="L22" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="N22" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O22" s="0" t="s">
+      <c r="O22" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="P22" s="0" t="s">
+      <c r="P22" s="10" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1258,34 +1310,34 @@
       <c r="B23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="K23" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="L23" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M23" s="0" t="n">
+      <c r="L23" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M23" s="10" t="n">
         <v>31</v>
       </c>
-      <c r="N23" s="0" t="s">
+      <c r="N23" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="O23" s="0" t="s">
+      <c r="O23" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="P23" s="0" t="s">
+      <c r="P23" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="Q23" s="0" t="s">
+      <c r="Q23" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="R23" s="0" t="n">
+      <c r="R23" s="10" t="n">
         <v>21</v>
       </c>
     </row>
@@ -1293,34 +1345,34 @@
       <c r="B24" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="K24" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="L24" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M24" s="0" t="n">
+      <c r="L24" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M24" s="10" t="n">
         <v>31</v>
       </c>
-      <c r="N24" s="0" t="s">
+      <c r="N24" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="O24" s="0" t="s">
+      <c r="O24" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="P24" s="0" t="s">
+      <c r="P24" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="Q24" s="0" t="s">
+      <c r="Q24" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="R24" s="0" t="n">
+      <c r="R24" s="10" t="n">
         <v>22</v>
       </c>
     </row>
@@ -1328,22 +1380,22 @@
       <c r="B25" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K25" s="0" t="n">
+      <c r="C25" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="L25" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N25" s="0" t="s">
+      <c r="L25" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="N25" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="O25" s="0" t="s">
+      <c r="O25" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="P25" s="0" t="s">
+      <c r="P25" s="10" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1351,31 +1403,31 @@
       <c r="B26" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K26" s="0" t="n">
+      <c r="C26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="L26" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M26" s="0" t="n">
+      <c r="L26" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M26" s="10" t="n">
         <v>31</v>
       </c>
-      <c r="N26" s="0" t="s">
+      <c r="N26" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="O26" s="0" t="s">
+      <c r="O26" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="P26" s="0" t="s">
+      <c r="P26" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="Q26" s="0" t="s">
+      <c r="Q26" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="R26" s="0" t="n">
+      <c r="R26" s="10" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1383,22 +1435,22 @@
       <c r="B27" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K27" s="0" t="n">
+      <c r="C27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" s="10" t="n">
         <v>26</v>
       </c>
-      <c r="L27" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N27" s="0" t="s">
+      <c r="L27" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="N27" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="O27" s="0" t="s">
+      <c r="O27" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="P27" s="0" t="s">
+      <c r="P27" s="10" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1406,13 +1458,13 @@
       <c r="B28" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="K28" s="0" t="n">
+      <c r="K28" s="10" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1420,13 +1472,13 @@
       <c r="B29" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K29" s="0" t="n">
+      <c r="C29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" s="10" t="n">
         <v>28</v>
       </c>
-      <c r="M29" s="0" t="n">
+      <c r="M29" s="10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1434,10 +1486,10 @@
       <c r="B30" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="K30" s="0" t="n">
+      <c r="K30" s="10" t="n">
         <v>29</v>
       </c>
     </row>
@@ -1445,13 +1497,13 @@
       <c r="B31" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K31" s="0" t="n">
+      <c r="C31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="M31" s="0" t="n">
+      <c r="M31" s="10" t="n">
         <v>71</v>
       </c>
     </row>
@@ -1459,13 +1511,13 @@
       <c r="B32" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K32" s="0" t="n">
+      <c r="C32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K32" s="10" t="n">
         <v>31</v>
       </c>
-      <c r="M32" s="0" t="n">
+      <c r="M32" s="10" t="n">
         <v>72</v>
       </c>
     </row>
@@ -1473,13 +1525,13 @@
       <c r="B33" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K33" s="0" t="n">
+      <c r="C33" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="10" t="n">
         <v>32</v>
       </c>
-      <c r="L33" s="0" t="n">
+      <c r="L33" s="10" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1487,13 +1539,13 @@
       <c r="B34" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K34" s="0" t="n">
+      <c r="C34" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="10" t="n">
         <v>33</v>
       </c>
-      <c r="L34" s="0" t="n">
+      <c r="L34" s="10" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1501,13 +1553,13 @@
       <c r="B35" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K35" s="0" t="n">
+      <c r="C35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" s="10" t="n">
         <v>34</v>
       </c>
-      <c r="M35" s="0" t="n">
+      <c r="M35" s="10" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1515,13 +1567,13 @@
       <c r="B36" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K36" s="0" t="n">
+      <c r="C36" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="M36" s="0" t="n">
+      <c r="M36" s="10" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1529,13 +1581,13 @@
       <c r="B37" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K37" s="0" t="n">
+      <c r="C37" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="10" t="n">
         <v>36</v>
       </c>
-      <c r="M37" s="0" t="n">
+      <c r="M37" s="10" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1543,13 +1595,13 @@
       <c r="B38" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K38" s="0" t="n">
+      <c r="C38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38" s="10" t="n">
         <v>37</v>
       </c>
-      <c r="L38" s="0" t="n">
+      <c r="L38" s="10" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1557,14 +1609,22 @@
       <c r="B39" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K39" s="0" t="n">
+      <c r="C39" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="10" t="n">
         <v>38</v>
       </c>
-      <c r="M39" s="0" t="n">
+      <c r="M39" s="10" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>